<commit_message>
Added smoke sanity report for Rhythm EMR version RTM_V2.1.8F
</commit_message>
<xml_diff>
--- a/Library/SmokeSanityTestCases_RTM.xlsx
+++ b/Library/SmokeSanityTestCases_RTM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -52,18 +52,12 @@
     <t>TC004</t>
   </si>
   <si>
-    <t>Radiology\TC001GenerateUSGReport.py</t>
-  </si>
-  <si>
     <t>TC005</t>
   </si>
   <si>
     <t>TC006</t>
   </si>
   <si>
-    <t>SanityTest</t>
-  </si>
-  <si>
     <t>ADT\TC011AdmissionDischargeTransferNoDeposit.py</t>
   </si>
   <si>
@@ -79,21 +73,12 @@
     <t>TC008</t>
   </si>
   <si>
-    <t>Reports\TC005IncomeSegregationReport.py</t>
-  </si>
-  <si>
     <t>TC009</t>
   </si>
   <si>
-    <t>TC010</t>
-  </si>
-  <si>
     <t>TC011</t>
   </si>
   <si>
-    <t>TC012</t>
-  </si>
-  <si>
     <t>Norun</t>
   </si>
   <si>
@@ -103,12 +88,6 @@
     <t>Manual Status</t>
   </si>
   <si>
-    <t>TC013</t>
-  </si>
-  <si>
-    <t>TC014</t>
-  </si>
-  <si>
     <t>Laboratory\TC005GenerateLabReport.py</t>
   </si>
   <si>
@@ -136,15 +115,6 @@
     <t>Patient\TC001PatientRegistrationPrintHealthCard.py</t>
   </si>
   <si>
-    <t>MedicalRecords\TC001createBirth&amp;DeathCertificate.py</t>
-  </si>
-  <si>
-    <t>MedicalRecords\Reports\TC001HospitalServiceSummaryReport.py</t>
-  </si>
-  <si>
-    <t>MedicalRecords\Reports\TC002InpatientMorbidityReport.py</t>
-  </si>
-  <si>
     <t>TC002</t>
   </si>
   <si>
@@ -152,9 +122,6 @@
   </si>
   <si>
     <t>Billing\OPbilling\TC002OPDbillingLabXray.py</t>
-  </si>
-  <si>
-    <t>Reports\TC011UserCollectionReport.py</t>
   </si>
   <si>
     <t>Patient</t>
@@ -547,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,7 +540,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -582,7 +549,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -590,7 +557,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -606,10 +573,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -618,17 +585,17 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -644,10 +611,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -663,10 +630,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -675,17 +642,17 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -694,17 +661,17 @@
         <v>0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
@@ -713,17 +680,17 @@
         <v>0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>6</v>
@@ -732,17 +699,17 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>6</v>
@@ -751,17 +718,17 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>6</v>
@@ -770,124 +737,10 @@
         <v>0</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -911,13 +764,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -925,7 +778,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -934,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -943,7 +796,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -952,7 +805,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -961,7 +814,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -970,7 +823,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -979,7 +832,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -988,7 +841,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2"/>
     </row>

</xml_diff>